<commit_message>
unlist embrace plus data
</commit_message>
<xml_diff>
--- a/app/static/example_data/embrace-plus_calendar_small.xlsx
+++ b/app/static/example_data/embrace-plus_calendar_small.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veerlevanleemput/Documents/Hypebright BV/Fivoor/wearalyze/app/static/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA4B6C8-0559-7E45-A7D4-BD2ADEC80C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2298CCE-4109-894B-A361-5F666684B016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37460" yWindow="4300" windowWidth="27640" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Spilled hot tea</t>
+  </si>
+  <si>
+    <t>Watching TV</t>
   </si>
 </sst>
 </file>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -494,6 +497,23 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45118</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>